<commit_message>
Modifica del file delle soluzioni di istanza ed aggiunta di soluzioni calcolate con l'esatto
</commit_message>
<xml_diff>
--- a/docs/MKP solutions.xlsx
+++ b/docs/MKP solutions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maxence\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giaco\IdeaProjects\KernelSearchGolinoCottiBeatrice\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202219D7-31BB-4778-9399-1D724A07E470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47461BCC-2D48-4997-8BC3-CBDEBFAAB180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="11" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2107" uniqueCount="2107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2112" uniqueCount="2110">
   <si>
     <t>Instance</t>
   </si>
@@ -6355,6 +6355,15 @@
   </si>
   <si>
     <t>_OUTPUT/random75_375_4_1000_1_20.txt_MULKNAP_EASY.txt</t>
+  </si>
+  <si>
+    <t>NOT OPT</t>
+  </si>
+  <si>
+    <t>KERNEL</t>
+  </si>
+  <si>
+    <t>O.F.</t>
   </si>
 </sst>
 </file>
@@ -6384,7 +6393,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -6420,11 +6429,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6449,9 +6482,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -6732,19 +6783,21 @@
   <dimension ref="A1:KH2106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="61" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.88671875" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.109375" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.44140625" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="7" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="55.21875" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="11.5546875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:142" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -6759,8 +6812,13 @@
       </c>
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="J1" s="12" t="s">
+        <v>2108</v>
+      </c>
+      <c r="K1" s="13"/>
+      <c r="L1" s="14"/>
+    </row>
+    <row r="2" spans="1:142" x14ac:dyDescent="0.3">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -6773,8 +6831,23 @@
       <c r="F2" s="8" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I2" s="10" t="s">
+        <v>2107</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>2109</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="EL2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:142" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
@@ -6793,8 +6866,15 @@
       <c r="F3" s="8">
         <v>9114</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I3" s="15" t="str">
+        <f>IF(D977=EL976,A977,"")</f>
+        <v>_OUTPUT/random30_90_4_1000_1_13.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+    </row>
+    <row r="4" spans="1:142" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>6</v>
       </c>
@@ -6813,8 +6893,15 @@
       <c r="F4" s="8">
         <v>8727</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I4" s="15" t="str">
+        <f>IF(D1345=EL1343,A1345,"")</f>
+        <v>_OUTPUT/random36_144_2_1000_1_20.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+    </row>
+    <row r="5" spans="1:142" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>7</v>
       </c>
@@ -6833,8 +6920,15 @@
       <c r="F5" s="8">
         <v>6422</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I5" s="15" t="str">
+        <f>IF(D1426=EL1424,A1426,"")</f>
+        <v>_OUTPUT/random45_135_3_1000_1_1.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+    </row>
+    <row r="6" spans="1:142" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>8</v>
       </c>
@@ -6853,8 +6947,15 @@
       <c r="F6" s="8">
         <v>7626</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I6" s="15" t="str">
+        <f>IF(D1437=EL1435,A1437,"")</f>
+        <v>_OUTPUT/random45_135_3_1000_1_12.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+    </row>
+    <row r="7" spans="1:142" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>9</v>
       </c>
@@ -6873,8 +6974,15 @@
       <c r="F7" s="8">
         <v>6782</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I7" s="15" t="str">
+        <f>IF(D1459=EL1458,A1459,"")</f>
+        <v>_OUTPUT/random45_135_4_1000_1_14.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+    </row>
+    <row r="8" spans="1:142" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>10</v>
       </c>
@@ -6893,8 +7001,15 @@
       <c r="F8" s="8">
         <v>6590</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I8" s="15" t="str">
+        <f>IF(D1505=EL1504,A1505,"")</f>
+        <v>_OUTPUT/random45_225_2_1000_1_20.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+    </row>
+    <row r="9" spans="1:142" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>11</v>
       </c>
@@ -6913,8 +7028,15 @@
       <c r="F9" s="8">
         <v>7077</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I9" s="15" t="str">
+        <f>IF(D1651=EL1649,A1651,"")</f>
+        <v>_OUTPUT/random50_300_2_1000_1_5.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+    </row>
+    <row r="10" spans="1:142" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>12</v>
       </c>
@@ -6933,8 +7055,15 @@
       <c r="F10" s="8">
         <v>6387</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I10" s="15" t="str">
+        <f>IF(D1787=EL1785,A1787,"")</f>
+        <v>_OUTPUT/random60_240_1_1000_1_1.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+    </row>
+    <row r="11" spans="1:142" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>13</v>
       </c>
@@ -6953,8 +7082,15 @@
       <c r="F11" s="8">
         <v>7915</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I11" s="15" t="str">
+        <f>IF(D1803=EL1802,A1803,"")</f>
+        <v>_OUTPUT/random60_240_1_1000_1_17.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+    </row>
+    <row r="12" spans="1:142" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>14</v>
       </c>
@@ -6973,8 +7109,15 @@
       <c r="F12" s="8">
         <v>8195</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I12" s="15" t="str">
+        <f>IF(D1805=EL1804,A1805,"")</f>
+        <v>_OUTPUT/random60_240_1_1000_1_19.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+    </row>
+    <row r="13" spans="1:142" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>15</v>
       </c>
@@ -6993,8 +7136,15 @@
       <c r="F13" s="8">
         <v>17936</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I13" s="15" t="str">
+        <f>IF(D1809=EL1808,A1809,"")</f>
+        <v>_OUTPUT/random60_240_2_1000_1_3.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+    </row>
+    <row r="14" spans="1:142" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>16</v>
       </c>
@@ -7013,8 +7163,15 @@
       <c r="F14" s="8">
         <v>16420</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I14" s="15" t="str">
+        <f>IF(D1810=EL1808,A1810,"")</f>
+        <v>_OUTPUT/random60_240_2_1000_1_4.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+    </row>
+    <row r="15" spans="1:142" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>17</v>
       </c>
@@ -7033,8 +7190,15 @@
       <c r="F15" s="8">
         <v>15466</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I15" s="15" t="str">
+        <f>IF(D1812=EL1810,A1812,"")</f>
+        <v>_OUTPUT/random60_240_2_1000_1_6.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+    </row>
+    <row r="16" spans="1:142" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>18</v>
       </c>
@@ -7053,8 +7217,15 @@
       <c r="F16" s="8">
         <v>17292</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I16" s="15" t="str">
+        <f>IF(D1814=EL1812,A1814,"")</f>
+        <v>_OUTPUT/random60_240_2_1000_1_8.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>19</v>
       </c>
@@ -7073,8 +7244,15 @@
       <c r="F17" s="8">
         <v>15534</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I17" s="15" t="str">
+        <f>IF(D1815=EL1814,A1815,"")</f>
+        <v>_OUTPUT/random60_240_2_1000_1_9.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>20</v>
       </c>
@@ -7093,8 +7271,15 @@
       <c r="F18" s="8">
         <v>16510</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I18" s="15" t="str">
+        <f>IF(D1816=EL1814,A1816,"")</f>
+        <v>_OUTPUT/random60_240_2_1000_1_10.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>21</v>
       </c>
@@ -7113,8 +7298,15 @@
       <c r="F19" s="8">
         <v>14434</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I19" s="15" t="str">
+        <f>IF(D1819=EL1818,A1819,"")</f>
+        <v>_OUTPUT/random60_240_2_1000_1_13.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>22</v>
       </c>
@@ -7133,8 +7325,15 @@
       <c r="F20" s="8">
         <v>16166</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I20" s="15" t="str">
+        <f>IF(D1821=EL1820,A1821,"")</f>
+        <v>_OUTPUT/random60_240_2_1000_1_15.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>23</v>
       </c>
@@ -7153,8 +7352,15 @@
       <c r="F21" s="8">
         <v>16444</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I21" s="15" t="str">
+        <f>IF(D1822=EL1820,A1822,"")</f>
+        <v>_OUTPUT/random60_240_2_1000_1_16.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>24</v>
       </c>
@@ -7173,8 +7379,15 @@
       <c r="F22" s="8">
         <v>17465</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I22" s="15" t="str">
+        <f>IF(D1823=EL1822,A1823,"")</f>
+        <v>_OUTPUT/random60_240_2_1000_1_17.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
         <v>25</v>
       </c>
@@ -7193,8 +7406,15 @@
       <c r="F23" s="8">
         <v>26596</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I23" s="15" t="str">
+        <f>IF(D1825=EL1824,A1825,"")</f>
+        <v>_OUTPUT/random60_240_2_1000_1_19.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
         <v>26</v>
       </c>
@@ -7213,8 +7433,15 @@
       <c r="F24" s="8">
         <v>23187</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I24" s="15" t="str">
+        <f>IF(D1827=EL1826,A1827,"")</f>
+        <v>_OUTPUT/random60_240_3_1000_1_1.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
         <v>27</v>
       </c>
@@ -7233,8 +7460,15 @@
       <c r="F25" s="8">
         <v>23630</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I25" s="15" t="str">
+        <f>IF(D1836=EL1835,A1836,"")</f>
+        <v>_OUTPUT/random60_240_3_1000_1_10.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
         <v>28</v>
       </c>
@@ -7253,8 +7487,15 @@
       <c r="F26" s="8">
         <v>24462</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I26" s="15" t="str">
+        <f>IF(D1837=EL1835,A1837,"")</f>
+        <v>_OUTPUT/random60_240_3_1000_1_11.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
         <v>29</v>
       </c>
@@ -7273,8 +7514,15 @@
       <c r="F27" s="8">
         <v>24611</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I27" s="15" t="str">
+        <f>IF(D1844=EL1843,A1844,"")</f>
+        <v>_OUTPUT/random60_240_3_1000_1_18.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J27" s="15"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
         <v>30</v>
       </c>
@@ -7293,8 +7541,15 @@
       <c r="F28" s="8">
         <v>25631</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I28" s="15" t="str">
+        <f>IF(D1867=EL1866,A1867,"")</f>
+        <v>_OUTPUT/random75_225_1_1000_1_1.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
         <v>31</v>
       </c>
@@ -7313,8 +7568,15 @@
       <c r="F29" s="8">
         <v>23653</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I29" s="15" t="str">
+        <f>IF(D1868=EL1866,A1868,"")</f>
+        <v>_OUTPUT/random75_225_1_1000_1_2.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="15"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
         <v>32</v>
       </c>
@@ -7333,8 +7595,15 @@
       <c r="F30" s="8">
         <v>24177</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I30" s="15" t="str">
+        <f>IF(D1884=EL1883,A1884,"")</f>
+        <v>_OUTPUT/random75_225_1_1000_1_18.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
         <v>33</v>
       </c>
@@ -7353,8 +7622,15 @@
       <c r="F31" s="8">
         <v>24403</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I31" s="15" t="str">
+        <f>IF(D1886=EL1885,A1886,"")</f>
+        <v>_OUTPUT/random75_225_1_1000_1_20.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="15"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
         <v>34</v>
       </c>
@@ -7373,8 +7649,15 @@
       <c r="F32" s="8">
         <v>26936</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I32" s="15" t="str">
+        <f>IF(D1890=EL1889,A1890,"")</f>
+        <v>_OUTPUT/random75_225_2_1000_1_4.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
         <v>35</v>
       </c>
@@ -7393,8 +7676,15 @@
       <c r="F33" s="8">
         <v>7613</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I33" s="15" t="str">
+        <f>IF(D1891=EL1889,A1891,"")</f>
+        <v>_OUTPUT/random75_225_2_1000_1_5.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
         <v>36</v>
       </c>
@@ -7413,8 +7703,15 @@
       <c r="F34" s="8">
         <v>5324</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I34" s="15" t="str">
+        <f>IF(D1899=EL1897,A1899,"")</f>
+        <v>_OUTPUT/random75_225_2_1000_1_13.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
         <v>37</v>
       </c>
@@ -7433,8 +7730,15 @@
       <c r="F35" s="8">
         <v>3300</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I35" s="15" t="str">
+        <f>IF(D1900=EL1899,A1900,"")</f>
+        <v>_OUTPUT/random75_225_2_1000_1_14.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
         <v>38</v>
       </c>
@@ -7453,8 +7757,15 @@
       <c r="F36" s="8">
         <v>4104</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I36" s="15" t="str">
+        <f>IF(D1903=EL1902,A1903,"")</f>
+        <v>_OUTPUT/random75_225_2_1000_1_17.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J36" s="15"/>
+      <c r="K36" s="15"/>
+      <c r="L36" s="15"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
         <v>39</v>
       </c>
@@ -7473,8 +7784,15 @@
       <c r="F37" s="8">
         <v>4045</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I37" s="15" t="str">
+        <f>IF(D1907=EL1906,A1907,"")</f>
+        <v>_OUTPUT/random75_225_3_1000_1_1.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J37" s="15"/>
+      <c r="K37" s="15"/>
+      <c r="L37" s="15"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
         <v>40</v>
       </c>
@@ -7493,8 +7811,15 @@
       <c r="F38" s="8">
         <v>5137</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I38" s="15" t="str">
+        <f>IF(D1909=EL1908,A1909,"")</f>
+        <v>_OUTPUT/random75_225_3_1000_1_3.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J38" s="15"/>
+      <c r="K38" s="15"/>
+      <c r="L38" s="15"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
         <v>41</v>
       </c>
@@ -7513,8 +7838,15 @@
       <c r="F39" s="8">
         <v>3744</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I39" s="15" t="str">
+        <f>IF(D1912=EL1910,A1912,"")</f>
+        <v>_OUTPUT/random75_225_3_1000_1_6.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J39" s="15"/>
+      <c r="K39" s="15"/>
+      <c r="L39" s="15"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="s">
         <v>42</v>
       </c>
@@ -7533,8 +7865,15 @@
       <c r="F40" s="8">
         <v>3675</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I40" s="15" t="str">
+        <f>IF(D1913=EL1912,A1913,"")</f>
+        <v>_OUTPUT/random75_225_3_1000_1_7.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J40" s="15"/>
+      <c r="K40" s="15"/>
+      <c r="L40" s="15"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
         <v>43</v>
       </c>
@@ -7553,8 +7892,15 @@
       <c r="F41" s="8">
         <v>3978</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I41" s="15" t="str">
+        <f>IF(D1914=EL1912,A1914,"")</f>
+        <v>_OUTPUT/random75_225_3_1000_1_8.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J41" s="15"/>
+      <c r="K41" s="15"/>
+      <c r="L41" s="15"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="8" t="s">
         <v>44</v>
       </c>
@@ -7573,8 +7919,15 @@
       <c r="F42" s="8">
         <v>5938</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I42" s="15" t="str">
+        <f>IF(D1915=EL1914,A1915,"")</f>
+        <v>_OUTPUT/random75_225_3_1000_1_9.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J42" s="15"/>
+      <c r="K42" s="15"/>
+      <c r="L42" s="15"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="8" t="s">
         <v>45</v>
       </c>
@@ -7593,8 +7946,15 @@
       <c r="F43" s="8">
         <v>17892</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I43" s="15" t="str">
+        <f>IF(D1916=EL1914,A1916,"")</f>
+        <v>_OUTPUT/random75_225_3_1000_1_10.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J43" s="15"/>
+      <c r="K43" s="15"/>
+      <c r="L43" s="15"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="8" t="s">
         <v>46</v>
       </c>
@@ -7613,8 +7973,15 @@
       <c r="F44" s="8">
         <v>14702</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I44" s="15" t="str">
+        <f>IF(D1917=EL1916,A1917,"")</f>
+        <v>_OUTPUT/random75_225_3_1000_1_11.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J44" s="15"/>
+      <c r="K44" s="15"/>
+      <c r="L44" s="15"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="8" t="s">
         <v>47</v>
       </c>
@@ -7633,8 +8000,15 @@
       <c r="F45" s="8">
         <v>14512</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I45" s="15" t="str">
+        <f>IF(D1919=EL1918,A1919,"")</f>
+        <v>_OUTPUT/random75_225_3_1000_1_13.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J45" s="15"/>
+      <c r="K45" s="15"/>
+      <c r="L45" s="15"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="8" t="s">
         <v>48</v>
       </c>
@@ -7653,8 +8027,15 @@
       <c r="F46" s="8">
         <v>16802</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I46" s="15" t="str">
+        <f>IF(D1921=EL1920,A1921,"")</f>
+        <v>_OUTPUT/random75_225_3_1000_1_15.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J46" s="15"/>
+      <c r="K46" s="15"/>
+      <c r="L46" s="15"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="8" t="s">
         <v>49</v>
       </c>
@@ -7673,8 +8054,15 @@
       <c r="F47" s="8">
         <v>14727</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I47" s="15" t="str">
+        <f>IF(D1923=EL1922,A1923,"")</f>
+        <v>_OUTPUT/random75_225_3_1000_1_17.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J47" s="15"/>
+      <c r="K47" s="15"/>
+      <c r="L47" s="15"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="8" t="s">
         <v>50</v>
       </c>
@@ -7693,8 +8081,15 @@
       <c r="F48" s="8">
         <v>15849</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I48" s="15" t="str">
+        <f>IF(D1924=EL1922,A1924,"")</f>
+        <v>_OUTPUT/random75_225_3_1000_1_18.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J48" s="15"/>
+      <c r="K48" s="15"/>
+      <c r="L48" s="15"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="8" t="s">
         <v>51</v>
       </c>
@@ -7713,8 +8108,15 @@
       <c r="F49" s="8">
         <v>13444</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I49" s="15" t="str">
+        <f>IF(D1927=EL1926,A1927,"")</f>
+        <v>_OUTPUT/random75_225_4_1000_1_1.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J49" s="15"/>
+      <c r="K49" s="15"/>
+      <c r="L49" s="15"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="8" t="s">
         <v>52</v>
       </c>
@@ -7733,8 +8135,15 @@
       <c r="F50" s="8">
         <v>14662</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I50" s="15" t="str">
+        <f>IF(D1928=EL1927,A1928,"")</f>
+        <v>_OUTPUT/random75_225_4_1000_1_2.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J50" s="15"/>
+      <c r="K50" s="15"/>
+      <c r="L50" s="15"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="s">
         <v>53</v>
       </c>
@@ -7753,8 +8162,15 @@
       <c r="F51" s="8">
         <v>15311</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I51" s="15" t="str">
+        <f>IF(D1929=EL1927,A1929,"")</f>
+        <v>_OUTPUT/random75_225_4_1000_1_3.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J51" s="15"/>
+      <c r="K51" s="15"/>
+      <c r="L51" s="15"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="8" t="s">
         <v>54</v>
       </c>
@@ -7773,8 +8189,15 @@
       <c r="F52" s="8">
         <v>16725</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I52" s="15" t="str">
+        <f>IF(D1930=EL1929,A1930,"")</f>
+        <v>_OUTPUT/random75_225_4_1000_1_4.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J52" s="15"/>
+      <c r="K52" s="15"/>
+      <c r="L52" s="15"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="8" t="s">
         <v>55</v>
       </c>
@@ -7793,8 +8216,15 @@
       <c r="F53" s="8">
         <v>26593</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I53" s="15" t="str">
+        <f>IF(D1931=EL1929,A1931,"")</f>
+        <v>_OUTPUT/random75_225_4_1000_1_5.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J53" s="15"/>
+      <c r="K53" s="15"/>
+      <c r="L53" s="15"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="8" t="s">
         <v>56</v>
       </c>
@@ -7813,8 +8243,15 @@
       <c r="F54" s="8">
         <v>23014</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I54" s="15" t="str">
+        <f>IF(D1932=EL1931,A1932,"")</f>
+        <v>_OUTPUT/random75_225_4_1000_1_6.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J54" s="15"/>
+      <c r="K54" s="15"/>
+      <c r="L54" s="15"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="8" t="s">
         <v>57</v>
       </c>
@@ -7833,8 +8270,15 @@
       <c r="F55" s="8">
         <v>23328</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I55" s="15" t="str">
+        <f>IF(D1933=EL1931,A1933,"")</f>
+        <v>_OUTPUT/random75_225_4_1000_1_7.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J55" s="15"/>
+      <c r="K55" s="15"/>
+      <c r="L55" s="15"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="8" t="s">
         <v>58</v>
       </c>
@@ -7853,8 +8297,15 @@
       <c r="F56" s="8">
         <v>24448</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I56" s="15" t="str">
+        <f>IF(D1934=EL1933,A1934,"")</f>
+        <v>_OUTPUT/random75_225_4_1000_1_8.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J56" s="15"/>
+      <c r="K56" s="15"/>
+      <c r="L56" s="15"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="8" t="s">
         <v>59</v>
       </c>
@@ -7873,8 +8324,15 @@
       <c r="F57" s="8">
         <v>24576</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I57" s="15" t="str">
+        <f>IF(D1935=EL1933,A1935,"")</f>
+        <v>_OUTPUT/random75_225_4_1000_1_9.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J57" s="15"/>
+      <c r="K57" s="15"/>
+      <c r="L57" s="15"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="8" t="s">
         <v>60</v>
       </c>
@@ -7893,8 +8351,15 @@
       <c r="F58" s="8">
         <v>25549</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I58" s="15" t="str">
+        <f>IF(D1936=EL1935,A1936,"")</f>
+        <v>_OUTPUT/random75_225_4_1000_1_10.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J58" s="15"/>
+      <c r="K58" s="15"/>
+      <c r="L58" s="15"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="8" t="s">
         <v>61</v>
       </c>
@@ -7913,8 +8378,15 @@
       <c r="F59" s="8">
         <v>23504</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I59" s="15" t="str">
+        <f>IF(D1937=EL1935,A1937,"")</f>
+        <v>_OUTPUT/random75_225_4_1000_1_11.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J59" s="15"/>
+      <c r="K59" s="15"/>
+      <c r="L59" s="15"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="8" t="s">
         <v>62</v>
       </c>
@@ -7933,8 +8405,15 @@
       <c r="F60" s="8">
         <v>24125</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I60" s="15" t="str">
+        <f>IF(D1938=EL1937,A1938,"")</f>
+        <v>_OUTPUT/random75_225_4_1000_1_12.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J60" s="15"/>
+      <c r="K60" s="15"/>
+      <c r="L60" s="15"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="8" t="s">
         <v>63</v>
       </c>
@@ -7953,8 +8432,15 @@
       <c r="F61" s="8">
         <v>24274</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I61" s="15" t="str">
+        <f>IF(D1939=EL1937,A1939,"")</f>
+        <v>_OUTPUT/random75_225_4_1000_1_13.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J61" s="15"/>
+      <c r="K61" s="15"/>
+      <c r="L61" s="15"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="8" t="s">
         <v>64</v>
       </c>
@@ -7973,8 +8459,15 @@
       <c r="F62" s="8">
         <v>26909</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I62" s="15" t="str">
+        <f>IF(D1940=EL1939,A1940,"")</f>
+        <v>_OUTPUT/random75_225_4_1000_1_14.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J62" s="15"/>
+      <c r="K62" s="15"/>
+      <c r="L62" s="15"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="8" t="s">
         <v>65</v>
       </c>
@@ -7993,8 +8486,15 @@
       <c r="F63" s="8">
         <v>5684</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I63" s="15" t="str">
+        <f>IF(D1941=EL1939,A1941,"")</f>
+        <v>_OUTPUT/random75_225_4_1000_1_15.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J63" s="15"/>
+      <c r="K63" s="15"/>
+      <c r="L63" s="15"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="8" t="s">
         <v>66</v>
       </c>
@@ -8013,8 +8513,15 @@
       <c r="F64" s="8">
         <v>5626</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I64" s="15" t="str">
+        <f>IF(D1942=EL1941,A1942,"")</f>
+        <v>_OUTPUT/random75_225_4_1000_1_16.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J64" s="15"/>
+      <c r="K64" s="15"/>
+      <c r="L64" s="15"/>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="8" t="s">
         <v>67</v>
       </c>
@@ -8033,8 +8540,15 @@
       <c r="F65" s="8">
         <v>4872</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I65" s="15" t="str">
+        <f>IF(D1943=EL1941,A1943,"")</f>
+        <v>_OUTPUT/random75_225_4_1000_1_17.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J65" s="15"/>
+      <c r="K65" s="15"/>
+      <c r="L65" s="15"/>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="8" t="s">
         <v>68</v>
       </c>
@@ -8053,8 +8567,15 @@
       <c r="F66" s="8">
         <v>6043</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I66" s="15" t="str">
+        <f>IF(D1944=EL1943,A1944,"")</f>
+        <v>_OUTPUT/random75_225_4_1000_1_18.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J66" s="15"/>
+      <c r="K66" s="15"/>
+      <c r="L66" s="15"/>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="8" t="s">
         <v>69</v>
       </c>
@@ -8073,8 +8594,15 @@
       <c r="F67" s="8">
         <v>5751</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I67" s="15" t="str">
+        <f>IF(D1945=EL1943,A1945,"")</f>
+        <v>_OUTPUT/random75_225_4_1000_1_19.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J67" s="15"/>
+      <c r="K67" s="15"/>
+      <c r="L67" s="15"/>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="8" t="s">
         <v>70</v>
       </c>
@@ -8093,8 +8621,15 @@
       <c r="F68" s="8">
         <v>5676</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I68" s="15" t="str">
+        <f>IF(D1946=EL1945,A1946,"")</f>
+        <v>_OUTPUT/random75_225_4_1000_1_20.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J68" s="15"/>
+      <c r="K68" s="15"/>
+      <c r="L68" s="15"/>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="8" t="s">
         <v>71</v>
       </c>
@@ -8113,8 +8648,15 @@
       <c r="F69" s="8">
         <v>4955</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I69" s="15" t="str">
+        <f>IF(D1960=EL1958,A1960,"")</f>
+        <v>_OUTPUT/random75_375_1_1000_1_14.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J69" s="15"/>
+      <c r="K69" s="15"/>
+      <c r="L69" s="15"/>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="8" t="s">
         <v>72</v>
       </c>
@@ -8133,8 +8675,15 @@
       <c r="F70" s="8">
         <v>5160</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I70" s="15" t="str">
+        <f>IF(D1968=EL1966,A1968,"")</f>
+        <v>_OUTPUT/random75_375_2_1000_1_2.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J70" s="15"/>
+      <c r="K70" s="15"/>
+      <c r="L70" s="15"/>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="8" t="s">
         <v>73</v>
       </c>
@@ -8153,8 +8702,15 @@
       <c r="F71" s="8">
         <v>6075</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I71" s="15" t="str">
+        <f>IF(D1970=EL1968,A1970,"")</f>
+        <v>_OUTPUT/random75_375_2_1000_1_4.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J71" s="15"/>
+      <c r="K71" s="15"/>
+      <c r="L71" s="15"/>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" s="8" t="s">
         <v>74</v>
       </c>
@@ -8173,8 +8729,15 @@
       <c r="F72" s="8">
         <v>6102</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I72" s="15" t="str">
+        <f>IF(D1973=EL1972,A1973,"")</f>
+        <v>_OUTPUT/random75_375_2_1000_1_7.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J72" s="15"/>
+      <c r="K72" s="15"/>
+      <c r="L72" s="15"/>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="8" t="s">
         <v>75</v>
       </c>
@@ -8193,8 +8756,15 @@
       <c r="F73" s="8">
         <v>12182</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I73" s="15" t="str">
+        <f>IF(D1975=EL1974,A1975,"")</f>
+        <v>_OUTPUT/random75_375_2_1000_1_9.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J73" s="15"/>
+      <c r="K73" s="15"/>
+      <c r="L73" s="15"/>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" s="8" t="s">
         <v>76</v>
       </c>
@@ -8213,8 +8783,15 @@
       <c r="F74" s="8">
         <v>12000</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I74" s="15" t="str">
+        <f>IF(D1977=EL1976,A1977,"")</f>
+        <v>_OUTPUT/random75_375_2_1000_1_11.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J74" s="15"/>
+      <c r="K74" s="15"/>
+      <c r="L74" s="15"/>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" s="8" t="s">
         <v>77</v>
       </c>
@@ -8233,8 +8810,15 @@
       <c r="F75" s="8">
         <v>12682</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I75" s="15" t="str">
+        <f>IF(D1981=EL1979,A1981,"")</f>
+        <v>_OUTPUT/random75_375_2_1000_1_15.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J75" s="15"/>
+      <c r="K75" s="15"/>
+      <c r="L75" s="15"/>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" s="8" t="s">
         <v>78</v>
       </c>
@@ -8253,8 +8837,15 @@
       <c r="F76" s="8">
         <v>13091</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I76" s="15" t="str">
+        <f>IF(D1982=EL1981,A1982,"")</f>
+        <v>_OUTPUT/random75_375_2_1000_1_16.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J76" s="15"/>
+      <c r="K76" s="15"/>
+      <c r="L76" s="15"/>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" s="8" t="s">
         <v>79</v>
       </c>
@@ -8273,8 +8864,15 @@
       <c r="F77" s="8">
         <v>11830</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I77" s="15" t="str">
+        <f>IF(D1983=EL1981,A1983,"")</f>
+        <v>_OUTPUT/random75_375_2_1000_1_17.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J77" s="15"/>
+      <c r="K77" s="15"/>
+      <c r="L77" s="15"/>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" s="8" t="s">
         <v>80</v>
       </c>
@@ -8293,8 +8891,15 @@
       <c r="F78" s="8">
         <v>13141</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I78" s="15" t="str">
+        <f>IF(D1984=EL1983,A1984,"")</f>
+        <v>_OUTPUT/random75_375_2_1000_1_18.txt_MULKNAP_EASY.txt</v>
+      </c>
+      <c r="J78" s="15"/>
+      <c r="K78" s="15"/>
+      <c r="L78" s="15"/>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" s="8" t="s">
         <v>81</v>
       </c>
@@ -8313,8 +8918,12 @@
       <c r="F79" s="8">
         <v>11671</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I79" s="11" t="str">
+        <f>IF(D2105=EL2104,A2105,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" s="8" t="s">
         <v>82</v>
       </c>
@@ -8332,6 +8941,10 @@
       </c>
       <c r="F80" s="8">
         <v>11632</v>
+      </c>
+      <c r="I80" s="11" t="str">
+        <f>IF(D2106=EL2104,A2106,"")</f>
+        <v/>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -10379,7 +10992,7 @@
       <c r="E183" s="3"/>
       <c r="F183" s="4"/>
       <c r="H183" s="4"/>
-      <c r="I183" s="2"/>
+      <c r="I183" s="11"/>
       <c r="J183" s="2"/>
       <c r="K183" s="2"/>
       <c r="L183" s="2"/>
@@ -17271,7 +17884,7 @@
         <v>13044</v>
       </c>
     </row>
-    <row r="657" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="657" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A657" s="8" t="s">
         <v>660</v>
       </c>
@@ -17285,7 +17898,7 @@
         <v>11017</v>
       </c>
     </row>
-    <row r="658" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="658" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A658" s="8" t="s">
         <v>661</v>
       </c>
@@ -17299,7 +17912,7 @@
         <v>12193</v>
       </c>
     </row>
-    <row r="659" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="659" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A659" s="8" t="s">
         <v>662</v>
       </c>
@@ -17313,7 +17926,7 @@
         <v>13880</v>
       </c>
     </row>
-    <row r="660" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="660" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A660" s="8" t="s">
         <v>663</v>
       </c>
@@ -17327,7 +17940,7 @@
         <v>12623</v>
       </c>
     </row>
-    <row r="661" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="661" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A661" s="8" t="s">
         <v>664</v>
       </c>
@@ -17341,7 +17954,7 @@
         <v>13558</v>
       </c>
     </row>
-    <row r="662" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="662" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A662" s="8" t="s">
         <v>665</v>
       </c>
@@ -17355,7 +17968,7 @@
         <v>8780</v>
       </c>
     </row>
-    <row r="663" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="663" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A663" s="8" t="s">
         <v>666</v>
       </c>
@@ -17369,15 +17982,19 @@
         <v>13428</v>
       </c>
     </row>
-    <row r="664" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="664" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A664" s="2"/>
       <c r="B664" s="2"/>
       <c r="C664" s="2"/>
       <c r="D664" s="2"/>
       <c r="E664" s="2"/>
       <c r="F664" s="2"/>
-    </row>
-    <row r="665" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I664" s="11"/>
+      <c r="J664" s="6"/>
+      <c r="K664" s="6"/>
+      <c r="L664" s="6"/>
+    </row>
+    <row r="665" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A665" s="8" t="s">
         <v>667</v>
       </c>
@@ -17391,7 +18008,7 @@
         <v>49513</v>
       </c>
     </row>
-    <row r="666" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="666" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A666" s="8" t="s">
         <v>668</v>
       </c>
@@ -17405,7 +18022,7 @@
         <v>49172</v>
       </c>
     </row>
-    <row r="667" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="667" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A667" s="8" t="s">
         <v>669</v>
       </c>
@@ -17419,7 +18036,7 @@
         <v>48847</v>
       </c>
     </row>
-    <row r="668" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="668" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A668" s="8" t="s">
         <v>670</v>
       </c>
@@ -17433,7 +18050,7 @@
         <v>45088</v>
       </c>
     </row>
-    <row r="669" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="669" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A669" s="8" t="s">
         <v>671</v>
       </c>
@@ -17447,7 +18064,7 @@
         <v>46350</v>
       </c>
     </row>
-    <row r="670" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="670" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A670" s="8" t="s">
         <v>672</v>
       </c>
@@ -17461,7 +18078,7 @@
         <v>45341</v>
       </c>
     </row>
-    <row r="671" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="671" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A671" s="8" t="s">
         <v>673</v>
       </c>
@@ -17475,7 +18092,7 @@
         <v>43725</v>
       </c>
     </row>
-    <row r="672" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="672" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A672" s="8" t="s">
         <v>674</v>
       </c>
@@ -23985,7 +24602,7 @@
         <v>23665</v>
       </c>
     </row>
-    <row r="1137" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1137" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1137" s="8" t="s">
         <v>1139</v>
       </c>
@@ -23999,7 +24616,7 @@
         <v>23539</v>
       </c>
     </row>
-    <row r="1138" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1138" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1138" s="8" t="s">
         <v>1140</v>
       </c>
@@ -24013,7 +24630,7 @@
         <v>25574</v>
       </c>
     </row>
-    <row r="1139" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1139" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1139" s="8" t="s">
         <v>1141</v>
       </c>
@@ -24027,7 +24644,7 @@
         <v>22467</v>
       </c>
     </row>
-    <row r="1140" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1140" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1140" s="8" t="s">
         <v>1142</v>
       </c>
@@ -24041,7 +24658,7 @@
         <v>24455</v>
       </c>
     </row>
-    <row r="1141" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1141" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1141" s="8" t="s">
         <v>1143</v>
       </c>
@@ -24055,7 +24672,7 @@
         <v>26563</v>
       </c>
     </row>
-    <row r="1142" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1142" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1142" s="8" t="s">
         <v>1144</v>
       </c>
@@ -24069,7 +24686,7 @@
         <v>23371</v>
       </c>
     </row>
-    <row r="1143" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1143" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1143" s="8" t="s">
         <v>1145</v>
       </c>
@@ -24083,7 +24700,7 @@
         <v>20463</v>
       </c>
     </row>
-    <row r="1144" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1144" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1144" s="8" t="s">
         <v>1146</v>
       </c>
@@ -24097,15 +24714,19 @@
         <v>23991</v>
       </c>
     </row>
-    <row r="1145" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1145" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1145" s="2"/>
       <c r="B1145" s="2"/>
       <c r="C1145" s="2"/>
       <c r="D1145" s="2"/>
       <c r="E1145" s="2"/>
       <c r="F1145" s="2"/>
-    </row>
-    <row r="1146" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I1145" s="11"/>
+      <c r="J1145" s="6"/>
+      <c r="K1145" s="6"/>
+      <c r="L1145" s="6"/>
+    </row>
+    <row r="1146" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1146" s="8" t="s">
         <v>1147</v>
       </c>
@@ -24119,7 +24740,7 @@
         <v>73462</v>
       </c>
     </row>
-    <row r="1147" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1147" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1147" s="8" t="s">
         <v>1148</v>
       </c>
@@ -24133,7 +24754,7 @@
         <v>71762</v>
       </c>
     </row>
-    <row r="1148" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1148" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1148" s="8" t="s">
         <v>1149</v>
       </c>
@@ -24147,7 +24768,7 @@
         <v>70909</v>
       </c>
     </row>
-    <row r="1149" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1149" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1149" s="8" t="s">
         <v>1150</v>
       </c>
@@ -24161,7 +24782,7 @@
         <v>67871</v>
       </c>
     </row>
-    <row r="1150" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1150" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1150" s="8" t="s">
         <v>1151</v>
       </c>
@@ -24175,7 +24796,7 @@
         <v>71215</v>
       </c>
     </row>
-    <row r="1151" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1151" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1151" s="8" t="s">
         <v>1152</v>
       </c>
@@ -24189,7 +24810,7 @@
         <v>68149</v>
       </c>
     </row>
-    <row r="1152" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1152" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1152" s="8" t="s">
         <v>1153</v>
       </c>
@@ -30699,7 +31320,7 @@
         <v>34870</v>
       </c>
     </row>
-    <row r="1617" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1617" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1617" s="8" t="s">
         <v>1618</v>
       </c>
@@ -30713,7 +31334,7 @@
         <v>38670</v>
       </c>
     </row>
-    <row r="1618" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1618" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1618" s="8" t="s">
         <v>1619</v>
       </c>
@@ -30727,7 +31348,7 @@
         <v>33297</v>
       </c>
     </row>
-    <row r="1619" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1619" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1619" s="8" t="s">
         <v>1620</v>
       </c>
@@ -30741,7 +31362,7 @@
         <v>39563</v>
       </c>
     </row>
-    <row r="1620" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1620" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1620" s="8" t="s">
         <v>1621</v>
       </c>
@@ -30755,7 +31376,7 @@
         <v>34963</v>
       </c>
     </row>
-    <row r="1621" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1621" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1621" s="8" t="s">
         <v>1622</v>
       </c>
@@ -30769,7 +31390,7 @@
         <v>38958</v>
       </c>
     </row>
-    <row r="1622" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1622" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1622" s="8" t="s">
         <v>1623</v>
       </c>
@@ -30783,7 +31404,7 @@
         <v>39406</v>
       </c>
     </row>
-    <row r="1623" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1623" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1623" s="8" t="s">
         <v>1624</v>
       </c>
@@ -30797,7 +31418,7 @@
         <v>31586</v>
       </c>
     </row>
-    <row r="1624" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1624" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1624" s="8" t="s">
         <v>1625</v>
       </c>
@@ -30811,7 +31432,7 @@
         <v>30047</v>
       </c>
     </row>
-    <row r="1625" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1625" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1625" s="8" t="s">
         <v>1626</v>
       </c>
@@ -30825,15 +31446,19 @@
         <v>29531</v>
       </c>
     </row>
-    <row r="1626" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1626" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1626" s="2"/>
       <c r="B1626" s="2"/>
       <c r="C1626" s="2"/>
       <c r="D1626" s="2"/>
       <c r="E1626" s="2"/>
       <c r="F1626" s="2"/>
-    </row>
-    <row r="1627" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I1626" s="11"/>
+      <c r="J1626" s="6"/>
+      <c r="K1626" s="6"/>
+      <c r="L1626" s="6"/>
+    </row>
+    <row r="1627" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1627" s="8" t="s">
         <v>1707</v>
       </c>
@@ -30847,7 +31472,7 @@
         <v>121806</v>
       </c>
     </row>
-    <row r="1628" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1628" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1628" s="8" t="s">
         <v>1708</v>
       </c>
@@ -30861,7 +31486,7 @@
         <v>119877</v>
       </c>
     </row>
-    <row r="1629" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1629" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1629" s="8" t="s">
         <v>1709</v>
       </c>
@@ -30875,7 +31500,7 @@
         <v>119806</v>
       </c>
     </row>
-    <row r="1630" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1630" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1630" s="8" t="s">
         <v>1710</v>
       </c>
@@ -30889,7 +31514,7 @@
         <v>115567</v>
       </c>
     </row>
-    <row r="1631" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1631" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1631" s="8" t="s">
         <v>1711</v>
       </c>
@@ -30903,7 +31528,7 @@
         <v>117204</v>
       </c>
     </row>
-    <row r="1632" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1632" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1632" s="8" t="s">
         <v>1712</v>
       </c>
@@ -37554,12 +38179,14 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:F1"/>
+    <mergeCell ref="J1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>